<commit_message>
reorganize folders, wave heights
</commit_message>
<xml_diff>
--- a/R Code and Analysis/output from r/2019 specimen name updates SCL.xlsx
+++ b/R Code and Analysis/output from r/2019 specimen name updates SCL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra\Documents\EliteNotebook\Jobs and Collaborations\Hakai\Community analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\Martone Lab\martone_calvert\R Code and Analysis\output from r\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46045F11-D302-4B88-9FF7-6143A28D0727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="6945"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 specimen name updates SCL" sheetId="1" r:id="rId1"/>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -974,20 +975,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="223.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1054,7 +1056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1082,7 +1084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1096,7 +1098,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1124,7 +1126,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1140,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1152,7 +1154,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1166,7 +1168,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1180,7 +1182,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1208,7 +1210,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1222,7 +1224,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1236,7 +1238,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1261,7 +1263,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1289,7 +1291,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1303,7 +1305,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1331,7 +1333,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1345,7 +1347,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1387,7 +1389,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1401,7 +1403,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1429,7 +1431,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1443,7 +1445,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>

</xml_diff>